<commit_message>
Added Averaging for duplicate samples
</commit_message>
<xml_diff>
--- a/ConcentrationNormalizer/EST BCA 20220923.xlsx
+++ b/ConcentrationNormalizer/EST BCA 20220923.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alani\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Python\GitHub Programs\PythonPrograms\ConcentrationNormalizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B2133D-C4BA-45C6-A452-60D9F9207ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99698580-8381-4473-B5A0-0051E0455EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4068" yWindow="1596" windowWidth="22092" windowHeight="14064" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>Method name: BCA</t>
   </si>
@@ -211,14 +211,38 @@
     <t>2022-09-23 16:12:26</t>
   </si>
   <si>
-    <t>IBR</t>
+    <t>D 1</t>
+  </si>
+  <si>
+    <t>D 2</t>
+  </si>
+  <si>
+    <t>D 3</t>
+  </si>
+  <si>
+    <t>247 1</t>
+  </si>
+  <si>
+    <t>247 2</t>
+  </si>
+  <si>
+    <t>247 3</t>
+  </si>
+  <si>
+    <t>IBR 1</t>
+  </si>
+  <si>
+    <t>IBR 2</t>
+  </si>
+  <si>
+    <t>IBR 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -231,6 +255,10 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -587,7 +615,7 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="Y38" sqref="Y38"/>
+      <selection activeCell="X43" sqref="X43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1236,31 +1264,31 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T34" s="1">
-        <v>247</v>
-      </c>
-      <c r="U34" s="1">
-        <v>247</v>
-      </c>
-      <c r="V34" s="1">
-        <v>247</v>
+        <v>65</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="X34" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="Z34" s="1"/>
     </row>
@@ -1310,31 +1338,31 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T35" s="1">
-        <v>247</v>
-      </c>
-      <c r="U35" s="1">
-        <v>247</v>
-      </c>
-      <c r="V35" s="1">
-        <v>247</v>
+        <v>65</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="Z35" s="1"/>
     </row>
@@ -1744,6 +1772,7 @@
       <c r="K46" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>